<commit_message>
Export can SelectDate, SSE can send (not tested with Forntend)
</commit_message>
<xml_diff>
--- a/exports/user_23_template.xlsx
+++ b/exports/user_23_template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Datetime</t>
   </si>
@@ -36,10 +36,7 @@
     <t>2024-07-03 14:30:00</t>
   </si>
   <si>
-    <t>100.50</t>
-  </si>
-  <si>
-    <t>Example transaction note REPLACE HERE</t>
+    <t>Example transaction note REPLACE HERE(28 Character)</t>
   </si>
   <si>
     <t>[tag_id,tag_id]</t>
@@ -545,17 +542,17 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>100.5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -575,13 +572,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -589,10 +586,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,10 +597,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -611,10 +608,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -622,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -633,10 +630,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -644,10 +641,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -655,10 +652,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -666,10 +663,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -677,10 +674,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -688,10 +685,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -699,10 +696,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -710,10 +707,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -721,10 +718,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -732,10 +729,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -743,10 +740,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -754,10 +751,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -777,10 +774,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -788,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>